<commit_message>
Diagrama de Casos de Uso
</commit_message>
<xml_diff>
--- a/Requisitos/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos/Requisitos e Casos de Uso.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
   <si>
     <t>NUM</t>
   </si>
@@ -128,6 +128,66 @@
   </si>
   <si>
     <t>Imprimir Itinerário</t>
+  </si>
+  <si>
+    <t>Listar Itens de uma Viagem</t>
+  </si>
+  <si>
+    <t>Adicionar Voo</t>
+  </si>
+  <si>
+    <t>Adicionar Hospedagem</t>
+  </si>
+  <si>
+    <t>Adicionar Trem</t>
+  </si>
+  <si>
+    <t>Adicionar Atração Turística</t>
+  </si>
+  <si>
+    <t>Adicionar Nota de Viagem</t>
+  </si>
+  <si>
+    <t>Gerenciar Voo</t>
+  </si>
+  <si>
+    <t>Gerenciar Hospedagem</t>
+  </si>
+  <si>
+    <t>Gerenciar Trem</t>
+  </si>
+  <si>
+    <t>Gerenciar Atração Turística</t>
+  </si>
+  <si>
+    <t>Gerenciar Nota de Viagem</t>
+  </si>
+  <si>
+    <t>Listar Viagens Futuras</t>
+  </si>
+  <si>
+    <t>Listar Histórico de Viagens</t>
+  </si>
+  <si>
+    <t>UC#</t>
+  </si>
+  <si>
+    <t>NOME DO UC</t>
+  </si>
+  <si>
+    <t>Servidor de e-mail</t>
+  </si>
+  <si>
+    <t>Autenticar Usuário</t>
+  </si>
+  <si>
+    <t>O usuário precisa se autenticar para utilizar as funcionalidades</t>
+  </si>
+  <si>
+    <t>Permitir que o usuário filtre os itens que são exibidos na lista de itens de uma viagem</t>
+  </si>
+  <si>
+    <t>Pesquisar Itens</t>
   </si>
 </sst>
 </file>
@@ -515,13 +575,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,6 +820,331 @@
         <v>21</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>13</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>16</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>17</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>18</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>19</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>21</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>22</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>25</v>
+      </c>
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>26</v>
+      </c>
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>